<commit_message>
data update may 2nd
</commit_message>
<xml_diff>
--- a/Egypt-data/Egypt.xlsx
+++ b/Egypt-data/Egypt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\R projects\COVID19\Egypt-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BD0879-2712-442B-8C90-F394960422FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C492043-DED2-492B-A450-5BDA771D8C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2040,6 +2040,197 @@
         <v>1780</v>
       </c>
     </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>43952</v>
+      </c>
+      <c r="B51">
+        <v>358</v>
+      </c>
+      <c r="C51">
+        <v>5895</v>
+      </c>
+      <c r="D51">
+        <v>1460</v>
+      </c>
+      <c r="E51">
+        <v>406</v>
+      </c>
+      <c r="F51">
+        <v>14</v>
+      </c>
+      <c r="G51">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>43953</v>
+      </c>
+      <c r="B52">
+        <v>298</v>
+      </c>
+      <c r="C52">
+        <v>6193</v>
+      </c>
+      <c r="D52">
+        <v>1522</v>
+      </c>
+      <c r="E52">
+        <v>415</v>
+      </c>
+      <c r="F52">
+        <v>9</v>
+      </c>
+      <c r="G52">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>43954</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>43955</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>43956</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>43957</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>43959</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>43960</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>43961</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>43962</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>43963</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>43965</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>43967</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>43968</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>43969</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>43970</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>43971</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>43972</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>43973</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>43974</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>43976</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>43979</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>43980</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>43981</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>43982</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
data update may 4th
</commit_message>
<xml_diff>
--- a/Egypt-data/Egypt.xlsx
+++ b/Egypt-data/Egypt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\R projects\COVID19\Egypt-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C492043-DED2-492B-A450-5BDA771D8C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373974CC-EDD6-44D6-A709-B83770FC34C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -885,7 +885,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2090,10 +2090,46 @@
       <c r="A53" s="1">
         <v>43954</v>
       </c>
+      <c r="B53">
+        <v>272</v>
+      </c>
+      <c r="C53">
+        <v>6465</v>
+      </c>
+      <c r="D53">
+        <v>1562</v>
+      </c>
+      <c r="E53">
+        <v>429</v>
+      </c>
+      <c r="F53">
+        <v>14</v>
+      </c>
+      <c r="G53">
+        <v>2041</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43955</v>
+      </c>
+      <c r="B54">
+        <v>348</v>
+      </c>
+      <c r="C54">
+        <v>6813</v>
+      </c>
+      <c r="D54">
+        <v>1632</v>
+      </c>
+      <c r="E54">
+        <v>436</v>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>2139</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
data update may 13th
</commit_message>
<xml_diff>
--- a/Egypt-data/Egypt.xlsx
+++ b/Egypt-data/Egypt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\R projects\COVID19\Egypt-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373974CC-EDD6-44D6-A709-B83770FC34C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DA4797-3DFA-47F0-8ECD-8FC8053636C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2136,45 +2136,207 @@
       <c r="A55" s="1">
         <v>43956</v>
       </c>
+      <c r="B55">
+        <v>388</v>
+      </c>
+      <c r="C55">
+        <v>7201</v>
+      </c>
+      <c r="D55">
+        <v>1730</v>
+      </c>
+      <c r="E55">
+        <v>452</v>
+      </c>
+      <c r="F55">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>2224</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>43957</v>
       </c>
+      <c r="B56">
+        <v>387</v>
+      </c>
+      <c r="C56">
+        <v>7588</v>
+      </c>
+      <c r="D56">
+        <v>1815</v>
+      </c>
+      <c r="E56">
+        <v>469</v>
+      </c>
+      <c r="F56">
+        <v>17</v>
+      </c>
+      <c r="G56">
+        <v>2314</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>43958</v>
       </c>
+      <c r="B57">
+        <v>393</v>
+      </c>
+      <c r="C57">
+        <v>7981</v>
+      </c>
+      <c r="D57">
+        <v>1887</v>
+      </c>
+      <c r="E57">
+        <v>482</v>
+      </c>
+      <c r="F57">
+        <v>13</v>
+      </c>
+      <c r="G57">
+        <v>2378</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>43959</v>
       </c>
+      <c r="B58">
+        <v>495</v>
+      </c>
+      <c r="C58">
+        <v>8476</v>
+      </c>
+      <c r="D58">
+        <v>1945</v>
+      </c>
+      <c r="E58">
+        <v>503</v>
+      </c>
+      <c r="F58">
+        <v>21</v>
+      </c>
+      <c r="G58">
+        <v>2416</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>43960</v>
       </c>
+      <c r="B59">
+        <v>488</v>
+      </c>
+      <c r="C59">
+        <v>8964</v>
+      </c>
+      <c r="D59">
+        <v>2002</v>
+      </c>
+      <c r="E59">
+        <v>514</v>
+      </c>
+      <c r="F59">
+        <v>11</v>
+      </c>
+      <c r="G59">
+        <v>2476</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>43961</v>
       </c>
+      <c r="B60">
+        <v>436</v>
+      </c>
+      <c r="C60">
+        <v>9400</v>
+      </c>
+      <c r="D60">
+        <v>2075</v>
+      </c>
+      <c r="E60">
+        <v>525</v>
+      </c>
+      <c r="F60">
+        <v>11</v>
+      </c>
+      <c r="G60">
+        <v>2556</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>43962</v>
       </c>
+      <c r="B61">
+        <v>346</v>
+      </c>
+      <c r="C61">
+        <v>9746</v>
+      </c>
+      <c r="D61">
+        <v>2172</v>
+      </c>
+      <c r="E61">
+        <v>533</v>
+      </c>
+      <c r="F61">
+        <v>8</v>
+      </c>
+      <c r="G61">
+        <v>2655</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>43963</v>
       </c>
+      <c r="B62">
+        <v>347</v>
+      </c>
+      <c r="C62">
+        <v>10093</v>
+      </c>
+      <c r="D62">
+        <v>2326</v>
+      </c>
+      <c r="E62">
+        <v>544</v>
+      </c>
+      <c r="F62">
+        <v>11</v>
+      </c>
+      <c r="G62">
+        <v>2811</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>43964</v>
+      </c>
+      <c r="B63">
+        <v>338</v>
+      </c>
+      <c r="C63">
+        <v>10431</v>
+      </c>
+      <c r="D63">
+        <v>2486</v>
+      </c>
+      <c r="E63">
+        <v>556</v>
+      </c>
+      <c r="F63">
+        <v>12</v>
+      </c>
+      <c r="G63">
+        <v>2980</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
data update jun 13th
</commit_message>
<xml_diff>
--- a/Egypt-data/Egypt.xlsx
+++ b/Egypt-data/Egypt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\R projects\COVID19\Egypt-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DA4797-3DFA-47F0-8ECD-8FC8053636C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90257A67-BE51-45AE-A08F-0BA406BBCD49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2343,91 +2343,765 @@
       <c r="A64" s="1">
         <v>43965</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>398</v>
+      </c>
+      <c r="C64">
+        <v>10829</v>
+      </c>
+      <c r="D64">
+        <v>2626</v>
+      </c>
+      <c r="E64">
+        <v>571</v>
+      </c>
+      <c r="F64">
+        <v>15</v>
+      </c>
+      <c r="G64">
+        <v>3133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>43966</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>399</v>
+      </c>
+      <c r="C65">
+        <v>11228</v>
+      </c>
+      <c r="D65">
+        <v>2799</v>
+      </c>
+      <c r="E65">
+        <v>592</v>
+      </c>
+      <c r="F65">
+        <v>21</v>
+      </c>
+      <c r="G65">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43967</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>491</v>
+      </c>
+      <c r="C66">
+        <v>11719</v>
+      </c>
+      <c r="D66">
+        <v>2950</v>
+      </c>
+      <c r="E66">
+        <v>612</v>
+      </c>
+      <c r="F66">
+        <v>20</v>
+      </c>
+      <c r="G66">
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>43968</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>510</v>
+      </c>
+      <c r="C67">
+        <v>12229</v>
+      </c>
+      <c r="D67">
+        <v>3172</v>
+      </c>
+      <c r="E67">
+        <v>630</v>
+      </c>
+      <c r="F67">
+        <v>18</v>
+      </c>
+      <c r="G67">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>43969</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>535</v>
+      </c>
+      <c r="C68">
+        <v>12764</v>
+      </c>
+      <c r="D68">
+        <v>3440</v>
+      </c>
+      <c r="E68">
+        <v>645</v>
+      </c>
+      <c r="F68">
+        <v>15</v>
+      </c>
+      <c r="G68">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>43970</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>720</v>
+      </c>
+      <c r="C69">
+        <v>13484</v>
+      </c>
+      <c r="D69">
+        <v>3742</v>
+      </c>
+      <c r="E69">
+        <v>659</v>
+      </c>
+      <c r="F69">
+        <v>14</v>
+      </c>
+      <c r="G69">
+        <v>4275</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>43971</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>745</v>
+      </c>
+      <c r="C70">
+        <v>14229</v>
+      </c>
+      <c r="D70">
+        <v>3994</v>
+      </c>
+      <c r="E70">
+        <v>680</v>
+      </c>
+      <c r="F70">
+        <v>21</v>
+      </c>
+      <c r="G70">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>43972</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>774</v>
+      </c>
+      <c r="C71">
+        <v>15003</v>
+      </c>
+      <c r="D71">
+        <v>4217</v>
+      </c>
+      <c r="E71">
+        <v>696</v>
+      </c>
+      <c r="F71">
+        <v>16</v>
+      </c>
+      <c r="G71">
+        <v>4798</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>43973</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>783</v>
+      </c>
+      <c r="C72">
+        <v>15786</v>
+      </c>
+      <c r="D72">
+        <v>4374</v>
+      </c>
+      <c r="E72">
+        <v>707</v>
+      </c>
+      <c r="F72">
+        <v>11</v>
+      </c>
+      <c r="G72">
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>43974</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>727</v>
+      </c>
+      <c r="C73">
+        <v>16513</v>
+      </c>
+      <c r="D73">
+        <v>4628</v>
+      </c>
+      <c r="E73">
+        <v>735</v>
+      </c>
+      <c r="F73">
+        <v>28</v>
+      </c>
+      <c r="G73">
+        <v>5192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>43975</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>752</v>
+      </c>
+      <c r="C74">
+        <v>17265</v>
+      </c>
+      <c r="D74">
+        <v>4807</v>
+      </c>
+      <c r="E74">
+        <v>764</v>
+      </c>
+      <c r="F74">
+        <v>29</v>
+      </c>
+      <c r="G74">
+        <v>5366</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>43976</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>702</v>
+      </c>
+      <c r="C75">
+        <v>17967</v>
+      </c>
+      <c r="D75">
+        <v>4900</v>
+      </c>
+      <c r="E75">
+        <v>783</v>
+      </c>
+      <c r="F75">
+        <v>19</v>
+      </c>
+      <c r="G75">
+        <v>5481</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>43977</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>789</v>
+      </c>
+      <c r="C76">
+        <v>18756</v>
+      </c>
+      <c r="D76">
+        <v>5027</v>
+      </c>
+      <c r="E76">
+        <v>797</v>
+      </c>
+      <c r="F76">
+        <v>14</v>
+      </c>
+      <c r="G76">
+        <v>5606</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>43978</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>910</v>
+      </c>
+      <c r="C77">
+        <v>19666</v>
+      </c>
+      <c r="D77">
+        <v>5205</v>
+      </c>
+      <c r="E77">
+        <v>816</v>
+      </c>
+      <c r="F77">
+        <v>19</v>
+      </c>
+      <c r="G77">
+        <v>5798</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>43979</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>1127</v>
+      </c>
+      <c r="C78">
+        <v>20793</v>
+      </c>
+      <c r="D78">
+        <v>5359</v>
+      </c>
+      <c r="E78">
+        <v>845</v>
+      </c>
+      <c r="F78">
+        <v>29</v>
+      </c>
+      <c r="G78">
+        <v>6019</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>43980</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>1289</v>
+      </c>
+      <c r="C79">
+        <v>22082</v>
+      </c>
+      <c r="D79">
+        <v>5511</v>
+      </c>
+      <c r="E79">
+        <v>879</v>
+      </c>
+      <c r="F79">
+        <v>34</v>
+      </c>
+      <c r="G79">
+        <v>6237</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>43981</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>1367</v>
+      </c>
+      <c r="C80">
+        <v>23449</v>
+      </c>
+      <c r="D80">
+        <v>5693</v>
+      </c>
+      <c r="E80">
+        <v>913</v>
+      </c>
+      <c r="F80">
+        <v>34</v>
+      </c>
+      <c r="G80">
+        <v>6456</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>43982</v>
       </c>
+      <c r="B81">
+        <v>1536</v>
+      </c>
+      <c r="C81">
+        <v>24985</v>
+      </c>
+      <c r="D81">
+        <v>6037</v>
+      </c>
+      <c r="E81">
+        <v>959</v>
+      </c>
+      <c r="F81">
+        <v>46</v>
+      </c>
+      <c r="G81">
+        <v>6810</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>43983</v>
+      </c>
+      <c r="B82">
+        <v>1399</v>
+      </c>
+      <c r="C82">
+        <v>26384</v>
+      </c>
+      <c r="D82">
+        <v>6447</v>
+      </c>
+      <c r="E82">
+        <v>1005</v>
+      </c>
+      <c r="F82">
+        <v>46</v>
+      </c>
+      <c r="G82">
+        <v>7149</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>43984</v>
+      </c>
+      <c r="B83">
+        <v>1152</v>
+      </c>
+      <c r="C83">
+        <v>27536</v>
+      </c>
+      <c r="D83">
+        <v>6827</v>
+      </c>
+      <c r="E83">
+        <v>1052</v>
+      </c>
+      <c r="F83">
+        <v>47</v>
+      </c>
+      <c r="G83">
+        <v>7642</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>43985</v>
+      </c>
+      <c r="B84">
+        <v>1079</v>
+      </c>
+      <c r="C84">
+        <v>28615</v>
+      </c>
+      <c r="D84">
+        <v>7350</v>
+      </c>
+      <c r="E84">
+        <v>1088</v>
+      </c>
+      <c r="F84">
+        <v>36</v>
+      </c>
+      <c r="G84">
+        <v>8371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>43986</v>
+      </c>
+      <c r="B85">
+        <v>1152</v>
+      </c>
+      <c r="C85">
+        <v>29767</v>
+      </c>
+      <c r="D85">
+        <v>7756</v>
+      </c>
+      <c r="E85">
+        <v>1126</v>
+      </c>
+      <c r="F85">
+        <v>38</v>
+      </c>
+      <c r="G85">
+        <v>8793</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>43987</v>
+      </c>
+      <c r="B86">
+        <v>1348</v>
+      </c>
+      <c r="C86">
+        <v>31115</v>
+      </c>
+      <c r="D86">
+        <v>8158</v>
+      </c>
+      <c r="E86">
+        <v>1166</v>
+      </c>
+      <c r="F86">
+        <v>40</v>
+      </c>
+      <c r="G86">
+        <v>9216</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>43988</v>
+      </c>
+      <c r="B87">
+        <v>1497</v>
+      </c>
+      <c r="C87">
+        <v>32612</v>
+      </c>
+      <c r="D87">
+        <v>8538</v>
+      </c>
+      <c r="E87">
+        <v>1198</v>
+      </c>
+      <c r="F87">
+        <v>32</v>
+      </c>
+      <c r="G87">
+        <v>9603</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>43989</v>
+      </c>
+      <c r="B88">
+        <v>1467</v>
+      </c>
+      <c r="C88">
+        <v>34079</v>
+      </c>
+      <c r="D88">
+        <v>8961</v>
+      </c>
+      <c r="E88">
+        <v>1237</v>
+      </c>
+      <c r="F88">
+        <v>39</v>
+      </c>
+      <c r="G88">
+        <v>10131</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>43990</v>
+      </c>
+      <c r="B89">
+        <v>1365</v>
+      </c>
+      <c r="C89">
+        <v>35444</v>
+      </c>
+      <c r="D89">
+        <v>9375</v>
+      </c>
+      <c r="E89">
+        <v>1271</v>
+      </c>
+      <c r="F89">
+        <v>34</v>
+      </c>
+      <c r="G89">
+        <v>10618</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>43991</v>
+      </c>
+      <c r="B90">
+        <v>1385</v>
+      </c>
+      <c r="C90">
+        <v>36829</v>
+      </c>
+      <c r="D90">
+        <v>9786</v>
+      </c>
+      <c r="E90">
+        <v>1306</v>
+      </c>
+      <c r="F90">
+        <v>35</v>
+      </c>
+      <c r="G90">
+        <v>11071</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>43992</v>
+      </c>
+      <c r="B91">
+        <v>1455</v>
+      </c>
+      <c r="C91">
+        <v>38284</v>
+      </c>
+      <c r="D91">
+        <v>10289</v>
+      </c>
+      <c r="E91">
+        <v>1342</v>
+      </c>
+      <c r="F91">
+        <v>36</v>
+      </c>
+      <c r="G91">
+        <v>11583</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>43993</v>
+      </c>
+      <c r="B92">
+        <v>1442</v>
+      </c>
+      <c r="C92">
+        <v>39726</v>
+      </c>
+      <c r="D92">
+        <v>10691</v>
+      </c>
+      <c r="E92">
+        <v>1377</v>
+      </c>
+      <c r="F92">
+        <v>35</v>
+      </c>
+      <c r="G92">
+        <v>12062</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="1">
+        <v>43994</v>
+      </c>
+      <c r="B93">
+        <v>1577</v>
+      </c>
+      <c r="C93">
+        <v>41303</v>
+      </c>
+      <c r="D93">
+        <v>11108</v>
+      </c>
+      <c r="E93">
+        <v>1422</v>
+      </c>
+      <c r="F93">
+        <v>45</v>
+      </c>
+      <c r="G93">
+        <v>12493</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="1">
+        <v>43995</v>
+      </c>
+      <c r="B94">
+        <v>1677</v>
+      </c>
+      <c r="C94">
+        <v>42980</v>
+      </c>
+      <c r="D94">
+        <v>11529</v>
+      </c>
+      <c r="E94">
+        <v>1484</v>
+      </c>
+      <c r="F94">
+        <v>62</v>
+      </c>
+      <c r="G94">
+        <v>12919</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>